<commit_message>
local-search(max-cut): latest stats saved
</commit_message>
<xml_diff>
--- a/asgn-3-local-search/mycodes/stats_local_search.xlsx
+++ b/asgn-3-local-search/mycodes/stats_local_search.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -430,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D8:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>